<commit_message>
changed lists, updated results and updated datafiles
</commit_message>
<xml_diff>
--- a/dashboard/Data/TFEC.xlsx
+++ b/dashboard/Data/TFEC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
   <si>
     <t>COM_CWH_BIO_001</t>
   </si>
@@ -286,6 +286,21 @@
   </si>
   <si>
     <t>Fuel</t>
+  </si>
+  <si>
+    <t>RES_CWH_KER_001</t>
+  </si>
+  <si>
+    <t>Residential solar thermal</t>
+  </si>
+  <si>
+    <t>RES_CWH_SOLAR</t>
+  </si>
+  <si>
+    <t>Water heating mainly</t>
+  </si>
+  <si>
+    <t>Solar</t>
   </si>
 </sst>
 </file>
@@ -643,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -785,7 +800,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -799,27 +814,27 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -828,49 +843,49 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -879,15 +894,15 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -896,32 +911,32 @@
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -930,24 +945,24 @@
         <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -955,13 +970,13 @@
         <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
         <v>54</v>
@@ -972,13 +987,13 @@
         <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
         <v>54</v>
@@ -989,7 +1004,7 @@
         <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
@@ -1006,13 +1021,13 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
@@ -1020,19 +1035,19 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1040,13 +1055,13 @@
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
         <v>27</v>
@@ -1054,10 +1069,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
         <v>24</v>
@@ -1066,7 +1081,7 @@
         <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1074,13 +1089,13 @@
         <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
         <v>70</v>
@@ -1088,19 +1103,19 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1108,7 +1123,7 @@
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
         <v>24</v>
@@ -1122,27 +1137,27 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
@@ -1151,15 +1166,15 @@
         <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
@@ -1168,15 +1183,15 @@
         <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
@@ -1185,32 +1200,32 @@
         <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
         <v>26</v>
@@ -1219,15 +1234,15 @@
         <v>50</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
@@ -1236,15 +1251,15 @@
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
@@ -1253,6 +1268,23 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all data files, model, results and lists updated
</commit_message>
<xml_diff>
--- a/dashboard/Data/TFEC.xlsx
+++ b/dashboard/Data/TFEC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="142">
   <si>
     <t>COM_CWH_BIO_001</t>
   </si>
@@ -366,9 +366,6 @@
     <t>IND_FOOD_NGS_001</t>
   </si>
   <si>
-    <t>IND_OTH_BIODSL_001</t>
-  </si>
-  <si>
     <t>IND_OTH_COA_001</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>Industry electricity</t>
   </si>
   <si>
-    <t>Industry biodiesel</t>
-  </si>
-  <si>
     <t>Industry diesel</t>
   </si>
   <si>
@@ -445,6 +439,12 @@
   </si>
   <si>
     <t>Oil</t>
+  </si>
+  <si>
+    <t>IND_OTH_BIO</t>
+  </si>
+  <si>
+    <t>TRA_CAR_NGS_001</t>
   </si>
 </sst>
 </file>
@@ -802,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1120,10 +1120,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1137,10 +1137,10 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1154,10 +1154,10 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1171,10 +1171,10 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1188,10 +1188,10 @@
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1205,10 +1205,10 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1222,10 +1222,10 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1239,10 +1239,10 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1256,10 +1256,10 @@
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1273,10 +1273,10 @@
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1290,10 +1290,10 @@
         <v>17</v>
       </c>
       <c r="D28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" t="s">
         <v>138</v>
-      </c>
-      <c r="E28" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1307,7 +1307,7 @@
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
         <v>46</v>
@@ -1324,7 +1324,7 @@
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
         <v>46</v>
@@ -1341,7 +1341,7 @@
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
         <v>46</v>
@@ -1358,7 +1358,7 @@
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E32" t="s">
         <v>46</v>
@@ -1375,7 +1375,7 @@
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
@@ -1392,7 +1392,7 @@
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
         <v>46</v>
@@ -1409,7 +1409,7 @@
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E35" t="s">
         <v>46</v>
@@ -1426,7 +1426,7 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E36" t="s">
         <v>56</v>
@@ -1443,7 +1443,7 @@
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E37" t="s">
         <v>56</v>
@@ -1460,7 +1460,7 @@
         <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E38" t="s">
         <v>56</v>
@@ -1477,7 +1477,7 @@
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E39" t="s">
         <v>34</v>
@@ -1494,7 +1494,7 @@
         <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E40" t="s">
         <v>34</v>
@@ -1511,7 +1511,7 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
@@ -1528,7 +1528,7 @@
         <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
@@ -1545,7 +1545,7 @@
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
@@ -1562,7 +1562,7 @@
         <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
@@ -1579,7 +1579,7 @@
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
@@ -1596,7 +1596,7 @@
         <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E46" t="s">
         <v>23</v>
@@ -1607,13 +1607,13 @@
         <v>100</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E47" t="s">
         <v>23</v>
@@ -1621,27 +1621,27 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="E48" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>18</v>
@@ -1655,10 +1655,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
         <v>18</v>
@@ -1667,15 +1667,15 @@
         <v>63</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
@@ -1684,15 +1684,15 @@
         <v>63</v>
       </c>
       <c r="E51" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -1706,10 +1706,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C53" t="s">
         <v>18</v>
@@ -1723,10 +1723,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
         <v>18</v>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C55" t="s">
         <v>18</v>
@@ -1757,10 +1757,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C56" t="s">
         <v>18</v>
@@ -1769,15 +1769,15 @@
         <v>63</v>
       </c>
       <c r="E56" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
         <v>18</v>
@@ -1791,10 +1791,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
         <v>18</v>
@@ -1808,10 +1808,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
         <v>18</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
         <v>18</v>
@@ -1842,10 +1842,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C61" t="s">
         <v>18</v>
@@ -1854,15 +1854,15 @@
         <v>63</v>
       </c>
       <c r="E61" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C62" t="s">
         <v>18</v>
@@ -1876,10 +1876,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
         <v>18</v>
@@ -1893,10 +1893,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
         <v>18</v>
@@ -1910,10 +1910,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
         <v>18</v>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C66" t="s">
         <v>18</v>
@@ -1939,15 +1939,15 @@
         <v>63</v>
       </c>
       <c r="E66" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C67" t="s">
         <v>18</v>
@@ -1956,15 +1956,15 @@
         <v>63</v>
       </c>
       <c r="E67" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
         <v>18</v>
@@ -1978,10 +1978,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
         <v>18</v>
@@ -1995,10 +1995,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C70" t="s">
         <v>18</v>
@@ -2012,10 +2012,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
@@ -2029,27 +2029,27 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E72" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
         <v>19</v>
@@ -2058,15 +2058,15 @@
         <v>42</v>
       </c>
       <c r="E73" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
         <v>19</v>
@@ -2075,15 +2075,15 @@
         <v>42</v>
       </c>
       <c r="E74" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
         <v>19</v>
@@ -2092,7 +2092,24 @@
         <v>42</v>
       </c>
       <c r="E75" t="s">
-        <v>141</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" t="s">
+        <v>42</v>
+      </c>
+      <c r="E76" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>